<commit_message>
VSC setting file added and generate db script file changed commited
</commit_message>
<xml_diff>
--- a/src/SQLDataAccess/SQLScriptFile/InsertDataScript/GenerateScript.xlsx
+++ b/src/SQLDataAccess/SQLScriptFile/InsertDataScript/GenerateScript.xlsx
@@ -1221,7 +1221,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F92" sqref="F1:F92"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1272,10 +1274,10 @@
       <c r="F2" t="str">
         <f>"INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (" &amp; A2 &amp; ", "&amp; B2 &amp; ", " &amp; C2 &amp; ", " &amp; D2 &amp; ", " &amp; E2 &amp; ")"</f>
-        <v>INSERT INTO dbo.tax_slab_details
- (id, tax_slab_id, from_amount, to_amount, percentage)
- (1, 1, null, 100000, 10)</v>
+VALUES (" &amp; A2 &amp; ", "&amp; B2 &amp; ", " &amp; C2 &amp; ", " &amp; D2 &amp; ", " &amp; E2 &amp; ")"</f>
+        <v>INSERT INTO dbo.tax_slab_details
+ (id, tax_slab_id, from_amount, to_amount, percentage)
+VALUES (1, 1, null, 100000, 10)</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1301,10 +1303,10 @@
       <c r="F3" t="str">
         <f t="shared" ref="F3:F66" si="0">"INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (" &amp; A3 &amp; ", "&amp; B3 &amp; ", " &amp; C3 &amp; ", " &amp; D3 &amp; ", " &amp; E3 &amp; ")"</f>
-        <v>INSERT INTO dbo.tax_slab_details
- (id, tax_slab_id, from_amount, to_amount, percentage)
- (2, 1, 100000, 200000, 11)</v>
+VALUES (" &amp; A3 &amp; ", "&amp; B3 &amp; ", " &amp; C3 &amp; ", " &amp; D3 &amp; ", " &amp; E3 &amp; ")"</f>
+        <v>INSERT INTO dbo.tax_slab_details
+ (id, tax_slab_id, from_amount, to_amount, percentage)
+VALUES (2, 1, 100000, 200000, 11)</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1330,7 +1332,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (3, 1, 200000, null, 12)</v>
+VALUES (3, 1, 200000, null, 12)</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1358,7 +1360,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (4, 2, null, 200000, 13)</v>
+VALUES (4, 2, null, 200000, 13)</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1386,7 +1388,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (5, 2, 200000, 300000, 14)</v>
+VALUES (5, 2, 200000, 300000, 14)</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1414,7 +1416,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (6, 2, 300000, null, 15)</v>
+VALUES (6, 2, 300000, null, 15)</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1442,7 +1444,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (7, 3, null, 300000, 16)</v>
+VALUES (7, 3, null, 300000, 16)</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1470,7 +1472,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (8, 3, 300000, 400000, 17)</v>
+VALUES (8, 3, 300000, 400000, 17)</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1498,7 +1500,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (9, 3, 400000, null, 18)</v>
+VALUES (9, 3, 400000, null, 18)</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1526,7 +1528,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (10, 4, null, 400000, 19)</v>
+VALUES (10, 4, null, 400000, 19)</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1554,7 +1556,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (11, 4, 400000, 500000, 20)</v>
+VALUES (11, 4, 400000, 500000, 20)</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1582,7 +1584,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (12, 4, 500000, null, 21)</v>
+VALUES (12, 4, 500000, null, 21)</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1610,7 +1612,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (13, 5, null, 500000, 22)</v>
+VALUES (13, 5, null, 500000, 22)</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1638,7 +1640,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (14, 5, 500000, 600000, 23)</v>
+VALUES (14, 5, 500000, 600000, 23)</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1666,7 +1668,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (15, 5, 600000, null, 24)</v>
+VALUES (15, 5, 600000, null, 24)</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1694,7 +1696,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (16, 6, null, 600000, 25)</v>
+VALUES (16, 6, null, 600000, 25)</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1722,7 +1724,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (17, 6, 600000, 700000, 26)</v>
+VALUES (17, 6, 600000, 700000, 26)</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1750,7 +1752,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (18, 6, 700000, null, 27)</v>
+VALUES (18, 6, 700000, null, 27)</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1778,7 +1780,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (19, 7, null, 700000, 28)</v>
+VALUES (19, 7, null, 700000, 28)</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1806,7 +1808,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (20, 7, 700000, 800000, 29)</v>
+VALUES (20, 7, 700000, 800000, 29)</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1834,7 +1836,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (21, 7, 800000, null, 30)</v>
+VALUES (21, 7, 800000, null, 30)</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1862,7 +1864,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (22, 8, null, 800000, 31)</v>
+VALUES (22, 8, null, 800000, 31)</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1890,7 +1892,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (23, 8, 800000, 900000, 32)</v>
+VALUES (23, 8, 800000, 900000, 32)</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1918,7 +1920,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (24, 8, 900000, null, 33)</v>
+VALUES (24, 8, 900000, null, 33)</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1946,7 +1948,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (25, 9, null, 900000, 34)</v>
+VALUES (25, 9, null, 900000, 34)</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1974,7 +1976,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (26, 9, 900000, 1000000, 35)</v>
+VALUES (26, 9, 900000, 1000000, 35)</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2002,7 +2004,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (27, 9, 1000000, null, 36)</v>
+VALUES (27, 9, 1000000, null, 36)</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2030,7 +2032,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (28, 10, null, 1000000, 37)</v>
+VALUES (28, 10, null, 1000000, 37)</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2058,7 +2060,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (29, 10, 1000000, 1100000, 38)</v>
+VALUES (29, 10, 1000000, 1100000, 38)</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2086,7 +2088,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (30, 10, 1100000, null, 39)</v>
+VALUES (30, 10, 1100000, null, 39)</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2114,7 +2116,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (31, 11, null, 1100000, 40)</v>
+VALUES (31, 11, null, 1100000, 40)</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2142,7 +2144,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (32, 11, 1100000, 1200000, 41)</v>
+VALUES (32, 11, 1100000, 1200000, 41)</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2170,7 +2172,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (33, 11, 1200000, null, 42)</v>
+VALUES (33, 11, 1200000, null, 42)</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2198,7 +2200,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (34, 12, null, 1200000, 43)</v>
+VALUES (34, 12, null, 1200000, 43)</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2226,7 +2228,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (35, 12, 1200000, 1300000, 44)</v>
+VALUES (35, 12, 1200000, 1300000, 44)</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2254,7 +2256,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (36, 12, 1300000, null, 45)</v>
+VALUES (36, 12, 1300000, null, 45)</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2282,7 +2284,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (37, 13, null, 1300000, 46)</v>
+VALUES (37, 13, null, 1300000, 46)</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2310,7 +2312,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (38, 13, 1300000, 1400000, 47)</v>
+VALUES (38, 13, 1300000, 1400000, 47)</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2338,7 +2340,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (39, 13, 1400000, null, 48)</v>
+VALUES (39, 13, 1400000, null, 48)</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2366,7 +2368,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (40, 14, null, 1400000, 49)</v>
+VALUES (40, 14, null, 1400000, 49)</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2394,7 +2396,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (41, 14, 1400000, 1500000, 50)</v>
+VALUES (41, 14, 1400000, 1500000, 50)</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2422,7 +2424,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (42, 14, 1500000, null, 51)</v>
+VALUES (42, 14, 1500000, null, 51)</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2450,7 +2452,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (43, 15, null, 1500000, 52)</v>
+VALUES (43, 15, null, 1500000, 52)</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2478,7 +2480,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (44, 15, 1500000, 1600000, 53)</v>
+VALUES (44, 15, 1500000, 1600000, 53)</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2506,7 +2508,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (45, 15, 1600000, null, 54)</v>
+VALUES (45, 15, 1600000, null, 54)</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2534,7 +2536,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (46, 16, null, 1600000, 55)</v>
+VALUES (46, 16, null, 1600000, 55)</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2562,7 +2564,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (47, 16, 1600000, 1700000, 56)</v>
+VALUES (47, 16, 1600000, 1700000, 56)</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2590,7 +2592,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (48, 16, 1700000, null, 57)</v>
+VALUES (48, 16, 1700000, null, 57)</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2618,7 +2620,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (49, 17, null, 1700000, 58)</v>
+VALUES (49, 17, null, 1700000, 58)</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2646,7 +2648,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (50, 17, 1700000, 1800000, 59)</v>
+VALUES (50, 17, 1700000, 1800000, 59)</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2674,7 +2676,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (51, 17, 1800000, null, 60)</v>
+VALUES (51, 17, 1800000, null, 60)</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2702,7 +2704,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (52, 18, null, 1800000, 61)</v>
+VALUES (52, 18, null, 1800000, 61)</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2730,7 +2732,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (53, 18, 1800000, 1900000, 62)</v>
+VALUES (53, 18, 1800000, 1900000, 62)</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2758,7 +2760,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (54, 18, 1900000, null, 63)</v>
+VALUES (54, 18, 1900000, null, 63)</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2786,7 +2788,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (55, 19, null, 1900000, 64)</v>
+VALUES (55, 19, null, 1900000, 64)</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2814,7 +2816,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (56, 19, 1900000, 2000000, 65)</v>
+VALUES (56, 19, 1900000, 2000000, 65)</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2842,7 +2844,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (57, 19, 2000000, null, 66)</v>
+VALUES (57, 19, 2000000, null, 66)</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2870,7 +2872,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (58, 20, null, 2000000, 67)</v>
+VALUES (58, 20, null, 2000000, 67)</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2898,7 +2900,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (59, 20, 2000000, 2100000, 68)</v>
+VALUES (59, 20, 2000000, 2100000, 68)</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2926,7 +2928,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (60, 20, 2100000, null, 69)</v>
+VALUES (60, 20, 2100000, null, 69)</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2954,7 +2956,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (61, 21, null, 2100000, 70)</v>
+VALUES (61, 21, null, 2100000, 70)</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2982,7 +2984,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (62, 21, 2100000, 2200000, 71)</v>
+VALUES (62, 21, 2100000, 2200000, 71)</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3010,7 +3012,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (63, 21, 2200000, null, 72)</v>
+VALUES (63, 21, 2200000, null, 72)</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -3038,7 +3040,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (64, 22, null, 2200000, 73)</v>
+VALUES (64, 22, null, 2200000, 73)</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3066,7 +3068,7 @@
         <f t="shared" si="0"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (65, 22, 2200000, 2300000, 74)</v>
+VALUES (65, 22, 2200000, 2300000, 74)</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3091,12 +3093,12 @@
         <v>75</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F91" si="6">"INSERT INTO dbo.tax_slab_details
- (id, tax_slab_id, from_amount, to_amount, percentage)
- (" &amp; A67 &amp; ", "&amp; B67 &amp; ", " &amp; C67 &amp; ", " &amp; D67 &amp; ", " &amp; E67 &amp; ")"</f>
-        <v>INSERT INTO dbo.tax_slab_details
- (id, tax_slab_id, from_amount, to_amount, percentage)
- (66, 22, 2300000, null, 75)</v>
+        <f t="shared" ref="F67:F92" si="6">"INSERT INTO dbo.tax_slab_details
+ (id, tax_slab_id, from_amount, to_amount, percentage)
+VALUES (" &amp; A67 &amp; ", "&amp; B67 &amp; ", " &amp; C67 &amp; ", " &amp; D67 &amp; ", " &amp; E67 &amp; ")"</f>
+        <v>INSERT INTO dbo.tax_slab_details
+ (id, tax_slab_id, from_amount, to_amount, percentage)
+VALUES (66, 22, 2300000, null, 75)</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3124,7 +3126,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (67, 23, null, 2300000, 76)</v>
+VALUES (67, 23, null, 2300000, 76)</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3152,7 +3154,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (68, 23, 2300000, 2400000, 77)</v>
+VALUES (68, 23, 2300000, 2400000, 77)</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3180,7 +3182,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (69, 23, 2400000, null, 78)</v>
+VALUES (69, 23, 2400000, null, 78)</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -3208,7 +3210,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (70, 24, null, 2400000, 79)</v>
+VALUES (70, 24, null, 2400000, 79)</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -3236,7 +3238,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (71, 24, 2400000, 2500000, 80)</v>
+VALUES (71, 24, 2400000, 2500000, 80)</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -3264,7 +3266,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (72, 24, 2500000, null, 81)</v>
+VALUES (72, 24, 2500000, null, 81)</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3292,7 +3294,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (73, 25, null, 2500000, 82)</v>
+VALUES (73, 25, null, 2500000, 82)</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -3320,7 +3322,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (74, 25, 2500000, 2600000, 83)</v>
+VALUES (74, 25, 2500000, 2600000, 83)</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -3348,7 +3350,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (75, 25, 2600000, null, 84)</v>
+VALUES (75, 25, 2600000, null, 84)</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -3376,7 +3378,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (76, 26, null, 2600000, 85)</v>
+VALUES (76, 26, null, 2600000, 85)</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -3404,7 +3406,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (77, 26, 2600000, 2700000, 86)</v>
+VALUES (77, 26, 2600000, 2700000, 86)</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3432,7 +3434,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (78, 26, 2700000, null, 87)</v>
+VALUES (78, 26, 2700000, null, 87)</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -3460,7 +3462,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (79, 27, null, 2700000, 88)</v>
+VALUES (79, 27, null, 2700000, 88)</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3488,7 +3490,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (80, 27, 2700000, 2800000, 89)</v>
+VALUES (80, 27, 2700000, 2800000, 89)</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3516,7 +3518,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (81, 27, 2800000, null, 90)</v>
+VALUES (81, 27, 2800000, null, 90)</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3544,7 +3546,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (82, 28, null, 2800000, 91)</v>
+VALUES (82, 28, null, 2800000, 91)</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -3572,7 +3574,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (83, 28, 2800000, 2900000, 92)</v>
+VALUES (83, 28, 2800000, 2900000, 92)</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3600,7 +3602,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (84, 28, 2900000, null, 93)</v>
+VALUES (84, 28, 2900000, null, 93)</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3628,7 +3630,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (85, 29, null, 2900000, 94)</v>
+VALUES (85, 29, null, 2900000, 94)</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -3656,7 +3658,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (86, 29, 2900000, 3000000, 95)</v>
+VALUES (86, 29, 2900000, 3000000, 95)</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3684,7 +3686,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (87, 29, 3000000, null, 96)</v>
+VALUES (87, 29, 3000000, null, 96)</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3712,7 +3714,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (88, 30, null, 3000000, 97)</v>
+VALUES (88, 30, null, 3000000, 97)</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3740,7 +3742,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (89, 30, 3000000, 3100000, 98)</v>
+VALUES (89, 30, 3000000, 3100000, 98)</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3768,7 +3770,7 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO dbo.tax_slab_details
  (id, tax_slab_id, from_amount, to_amount, percentage)
- (90, 30, 3100000, null, 99)</v>
+VALUES (90, 30, 3100000, null, 99)</v>
       </c>
     </row>
     <row r="92" spans="1:6">

</xml_diff>